<commit_message>
Update relevant documents with ~new/modified data
</commit_message>
<xml_diff>
--- a/DEMO_Radar.xlsx
+++ b/DEMO_Radar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fraunhofer.sharepoint.com/sites/TwinEU/Freigegebene Dokumente/WP3 Open Architecture for DT/T3.2/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="235" documentId="8_{2F75597A-2F00-0741-A778-D58A6DA629B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08A3F0C8-CD37-4EFB-B0E7-D516789EFD21}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{2F75597A-2F00-0741-A778-D58A6DA629B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44AB17B2-5CEF-4BE0-A442-08BAE48ABEDD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{93225E68-5AF0-2D40-91C0-91E1B9392F1F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{93225E68-5AF0-2D40-91C0-91E1B9392F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="DEMO WP5-CYBERSECURITY" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="144">
   <si>
     <t>Demonstrations of digital twinning for cyber-physical grid resilience</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>DT-SC&amp;PG-08</t>
+  </si>
+  <si>
+    <t>SLO02</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6310BE7-D968-BA44-AA58-3D3A5EF68010}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1339,7 +1342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E555F5-D9A5-8144-92A3-A1F89BA5FAE6}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1598,7 +1603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6592B94E-1467-2247-92C2-2331B56B6F58}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1759,7 +1766,7 @@
         <v>81</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>122</v>
@@ -1788,7 +1795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0E4DB3-BC65-465E-B959-36DC944F524E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1922,6 +1931,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010050B7A9603DF1A244B8132CE1C1B398A8" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a440459976170ea38fb7eb2e040ba179">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa" xmlns:ns3="6eb2050a-b6f7-4b0c-983c-e4078fb34326" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba382d81cd35db01624f0cbef7b1ab06" ns2:_="" ns3:_="">
     <xsd:import namespace="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa"/>
@@ -2156,15 +2174,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2177,6 +2186,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA1AB16B-69E7-43DA-8031-8031C51525BA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D35949-7414-4C08-9C49-36248DC50256}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2195,27 +2212,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA1AB16B-69E7-43DA-8031-8031C51525BA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36B192F0-A57E-435C-9C72-9692E1A65D61}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="6eb2050a-b6f7-4b0c-983c-e4078fb34326"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add apply latest changes to FURs and non-FURs based on updated specs
</commit_message>
<xml_diff>
--- a/DEMO_Radar.xlsx
+++ b/DEMO_Radar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\projects\TwinEU\WP3\T3.2\!GitHub-Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\projects\TwinEU\WP3\T3.2\!GitHub-Documents\T3.2_Functional_specifications_of_pan-European_DT_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E128F0B3-3707-40E6-9749-15B033525F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51A99D7B-58D7-48C2-A587-C043609D0FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{93225E68-5AF0-2D40-91C0-91E1B9392F1F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{93225E68-5AF0-2D40-91C0-91E1B9392F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="DEMO WP5-CYBERSECURITY" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="144">
   <si>
     <t>Demonstrations of digital twinning for cyber-physical grid resilience</t>
   </si>
@@ -413,9 +413,6 @@
     <t>Slovenian</t>
   </si>
   <si>
-    <t>SLO01</t>
-  </si>
-  <si>
     <t>DT-O&amp;M-08</t>
   </si>
   <si>
@@ -429,9 +426,6 @@
   </si>
   <si>
     <t>Hungarian</t>
-  </si>
-  <si>
-    <t>HU01</t>
   </si>
   <si>
     <t>There will be 2 more UCs in the Hungarian DEMO (UC2 and UC3). This work of WP6.8 can be be integral part of HUN UC2 or 3. This can be fixed when the 2 more UCs are in later version.</t>
@@ -480,9 +474,6 @@
     <t>7.3</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>not in T2.4 folder (just one UC so far)</t>
   </si>
   <si>
@@ -602,15 +593,41 @@
     <t>Leveraging the integrated Iberian DT continuum, a data-driven distributed robust optimisation approach will be applied in order to compute the ATC for the day-ahead and intraday market drawing probabilistic scenarios of VRE generation and grid contingencies to optimize strategies using the DT and compare with BAU. A properly tunned DT of a large multi-area control system (using the Iberian system as case-study), capable of providing the dynamic behaviour assessment, will be used to enable the identification of the type and volume and characterization of frequency ancillary services (including innovative ones like FFR, virtual inertia), which involves a set of new players like synchronous condensers, power electronic converts from batteries, power converters from RES generating units, pumps from reversible hydro power stations and dynamic load responses (EV charging and also hydrogen electrolysers). It will also address the problem of the optimum dimensioning and location of grid forming converters in an equivalent Iberian system for grid scenarios of 2030 and 2040 with large scale integration of power converters and reduced number of synchronous units.</t>
   </si>
   <si>
-    <r>
-      <rPr>
+    <t>DT-SC&amp;PG-05</t>
+  </si>
+  <si>
+    <t>DT-SC&amp;PG-06</t>
+  </si>
+  <si>
+    <t>DT-SC&amp;PG-07</t>
+  </si>
+  <si>
+    <t>DT-SC&amp;PG-08</t>
+  </si>
+  <si>
+    <r>
+      <t>Ib03,</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Ib03, Ib13, Ib14, Ib15, </t>
+      <t xml:space="preserve"> Ib13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ib10, </t>
     </r>
     <r>
       <rPr>
@@ -621,6 +638,48 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Ib14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ib11, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ib12, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Ib17</t>
     </r>
     <r>
@@ -631,29 +690,130 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Ib16</t>
-    </r>
-  </si>
-  <si>
-    <t>DT-SC&amp;PG-05</t>
-  </si>
-  <si>
-    <t>DT-SC&amp;PG-06</t>
-  </si>
-  <si>
-    <t>DT-SC&amp;PG-07</t>
-  </si>
-  <si>
-    <t>DT-SC&amp;PG-08</t>
-  </si>
-  <si>
-    <t>SLO02</t>
-  </si>
-  <si>
-    <t>Ib01, Ib12, Ib05, Ib06, Ib07, Ib08, Ib09, Ib10, Ib11, Ib12, Ib17</t>
-  </si>
-  <si>
-    <t>Ib03, Ib13, Ib14, Ib15, Ib16</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Ib13</t>
+    </r>
+  </si>
+  <si>
+    <t>SLO-BUC-02</t>
+  </si>
+  <si>
+    <t>Hu01</t>
+  </si>
+  <si>
+    <t>HU02, Hu03</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ib01, Ib04, Ib12, Ib05, Ib06, Ib07, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib08, Ib09, Ib10,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ib08, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Ib09, </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ib17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Ib14</t>
+    </r>
+  </si>
+  <si>
+    <t>SLO-BUC-01, SLO-BUC-03</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6310BE7-D968-BA44-AA58-3D3A5EF68010}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1315,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E555F5-D9A5-8144-92A3-A1F89BA5FAE6}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1520,44 +1680,44 @@
         <v>81</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>82</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="160" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="240" x14ac:dyDescent="0.4">
       <c r="B10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
@@ -1576,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6592B94E-1467-2247-92C2-2331B56B6F58}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1595,7 +1755,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
@@ -1621,96 +1781,96 @@
     </row>
     <row r="2" spans="1:8" ht="112" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="159" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="80" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D5" s="5">
         <v>7.5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="96" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D6" s="2">
         <v>7.6</v>
@@ -1719,18 +1879,18 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="80" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2">
         <v>7.7</v>
@@ -1739,20 +1899,20 @@
         <v>81</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1768,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0E4DB3-BC65-465E-B959-36DC944F524E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1787,7 +1947,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
@@ -1813,13 +1973,13 @@
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D2" s="2">
         <v>8.1999999999999993</v>
@@ -1828,21 +1988,21 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="80" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D3" s="2">
         <v>8.3000000000000007</v>
@@ -1851,18 +2011,18 @@
         <v>21</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="224" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D4" s="2">
         <v>8.4</v>
@@ -1871,27 +2031,27 @@
         <v>21</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1904,14 +2064,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6eb2050a-b6f7-4b0c-983c-e4078fb34326" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2150,27 +2308,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6eb2050a-b6f7-4b0c-983c-e4078fb34326" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36B192F0-A57E-435C-9C72-9692E1A65D61}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA1AB16B-69E7-43DA-8031-8031C51525BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6eb2050a-b6f7-4b0c-983c-e4078fb34326"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2195,9 +2346,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA1AB16B-69E7-43DA-8031-8031C51525BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36B192F0-A57E-435C-9C72-9692E1A65D61}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98aa5c30-0ca6-4ff6-9f27-712b5f6a60fa"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6eb2050a-b6f7-4b0c-983c-e4078fb34326"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>